<commit_message>
Se corrige azimut, hace falta revisar coordenadas
</commit_message>
<xml_diff>
--- a/basePolCerrada.xlsx
+++ b/basePolCerrada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoda\Desktop\Materias U\Materias 5 semestre\Ing de software\proyecto_ing_software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA99E096-1244-414F-93E9-8C7ABD20BC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BFB826-4FF0-4CB2-ADE0-8067773EF1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{CF3408B8-5A54-4B9D-A942-2992D31A9869}"/>
+    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7850" xr2:uid="{CF3408B8-5A54-4B9D-A942-2992D31A9869}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Δ</t>
   </si>
@@ -49,12 +49,6 @@
     <t>Obs.</t>
   </si>
   <si>
-    <t>FS</t>
-  </si>
-  <si>
-    <t>GP</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -65,6 +59,15 @@
   </si>
   <si>
     <t>D3</t>
+  </si>
+  <si>
+    <t>CT21</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>CT20</t>
   </si>
 </sst>
 </file>
@@ -635,16 +638,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80E0E97-3671-4E1A-8C43-1E9976CF96B4}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -652,7 +655,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -661,12 +664,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5">
         <v>0</v>
@@ -674,25 +677,25 @@
       <c r="D2" s="4"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3">
-        <v>2175112</v>
+        <v>2364556</v>
       </c>
       <c r="D3" s="2">
-        <v>12.954000000000001</v>
+        <v>70.811000000000007</v>
       </c>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -700,25 +703,25 @@
       <c r="D4" s="2"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>2652502</v>
+        <v>2813648</v>
       </c>
       <c r="D5" s="2">
-        <v>32.292000000000002</v>
+        <v>65.650999999999996</v>
       </c>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -726,25 +729,25 @@
       <c r="D6" s="2"/>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3">
-        <v>3162954</v>
+        <v>3063251</v>
       </c>
       <c r="D7" s="2">
-        <v>30.556000000000001</v>
+        <v>86.344999999999999</v>
       </c>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -752,89 +755,79 @@
       <c r="D8" s="2"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3">
-        <v>2592835</v>
-      </c>
-      <c r="D9" s="2">
-        <v>13.816000000000001</v>
-      </c>
+        <v>750445</v>
+      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="12"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="3">
         <v>0</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14"/>
-      <c r="B11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="16">
-        <v>204512</v>
-      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="15"/>
       <c r="E11" s="17"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C27" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se genera archivo exce hasta coordenadas hace falta generar el resto de listas
</commit_message>
<xml_diff>
--- a/basePolCerrada.xlsx
+++ b/basePolCerrada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoda\Desktop\Materias U\Materias 5 semestre\Ing de software\proyecto_ing_software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BFB826-4FF0-4CB2-ADE0-8067773EF1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5D8333-5BB5-451B-B00E-03A667F80659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7850" xr2:uid="{CF3408B8-5A54-4B9D-A942-2992D31A9869}"/>
+    <workbookView xWindow="372" yWindow="360" windowWidth="19152" windowHeight="10764" xr2:uid="{CF3408B8-5A54-4B9D-A942-2992D31A9869}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -246,56 +246,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -318,10 +273,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,18 +587,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80E0E97-3671-4E1A-8C43-1E9976CF96B4}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -664,7 +615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>8</v>
       </c>
@@ -677,7 +628,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -690,7 +641,7 @@
       </c>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
@@ -703,7 +654,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -716,7 +667,7 @@
       </c>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
@@ -729,7 +680,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -742,7 +693,7 @@
       </c>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>8</v>
       </c>
@@ -755,7 +706,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -766,69 +717,53 @@
       <c r="D9" s="2"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="13"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se deja listo pal parcial ahora si
</commit_message>
<xml_diff>
--- a/basePolCerrada.xlsx
+++ b/basePolCerrada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoda\Desktop\Materias U\Materias 5 semestre\Ing de software\proyecto_ing_software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6915E6F-14DC-48F2-8A1D-C01EC4A61803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBD9612-557F-444C-A608-B5EE40D64D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="348" windowWidth="19152" windowHeight="10764" xr2:uid="{CF3408B8-5A54-4B9D-A942-2992D31A9869}"/>
+    <workbookView xWindow="7008" yWindow="3180" windowWidth="19152" windowHeight="10764" xr2:uid="{CF3408B8-5A54-4B9D-A942-2992D31A9869}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Δ</t>
   </si>
@@ -61,13 +61,13 @@
     <t>D3</t>
   </si>
   <si>
-    <t>CT21</t>
-  </si>
-  <si>
-    <t>C20</t>
-  </si>
-  <si>
-    <t>CT20</t>
+    <t>CD20</t>
+  </si>
+  <si>
+    <t>CD17</t>
+  </si>
+  <si>
+    <t>D4</t>
   </si>
 </sst>
 </file>
@@ -109,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -246,11 +246,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -273,6 +284,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,7 +602,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,7 +632,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5">
         <v>0</v>
@@ -634,10 +646,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="3">
-        <v>2364556</v>
+        <v>2573013</v>
       </c>
       <c r="D3" s="2">
-        <v>70.811000000000007</v>
+        <v>94.028000000000006</v>
       </c>
       <c r="E3" s="13"/>
     </row>
@@ -660,10 +672,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>2813648</v>
+        <v>2435020</v>
       </c>
       <c r="D5" s="2">
-        <v>65.650999999999996</v>
+        <v>67.811000000000007</v>
       </c>
       <c r="E5" s="13"/>
     </row>
@@ -686,16 +698,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="3">
-        <v>3063251</v>
+        <v>2582451</v>
       </c>
       <c r="D7" s="2">
-        <v>86.344999999999999</v>
+        <v>61.104999999999997</v>
       </c>
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -709,25 +721,56 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2635757</v>
+      </c>
+      <c r="D9" s="2">
+        <v>68.375</v>
+      </c>
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1934253</v>
+      </c>
+      <c r="D11">
+        <v>56.484000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3">
-        <v>750445</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="1"/>
+      <c r="C13" s="1">
+        <v>423317</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>

</xml_diff>